<commit_message>
Modificar recaudaciones y remuneraciones
Se cambiaron las plantillas de recaudacion y remuneracion. Se agrego el concepto "Tasa Vial" a recaudacion y la columna "legajo" a remuneracion
</commit_message>
<xml_diff>
--- a/src/assets/plantillas/plantilla_recaudaciones.xlsx
+++ b/src/assets/plantillas/plantilla_recaudaciones.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OVIF\INFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A241955-965C-4D1C-9F16-5B2DB09EF6DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46FC3637-146A-4276-8372-1529E1C75B55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{356A1D58-5960-4CD7-A239-7EF8257EA826}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="plantilla_recaudaciones" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DatosExternos_1" localSheetId="0" hidden="1">plantilla_recaudaciones!$A$1:$C$9</definedName>
+    <definedName name="DatosExternos_1" localSheetId="0" hidden="1">plantilla_recaudaciones!$A$1:$C$10</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>cod_concepto</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t>Otros</t>
+  </si>
+  <si>
+    <t>Tasa Vial</t>
   </si>
 </sst>
 </file>
@@ -206,8 +209,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FAEA9955-847F-4766-AEEA-E6C31E526FE4}" name="plantilla_recaudaciones" displayName="plantilla_recaudaciones" ref="A1:C9" tableType="queryTable" totalsRowShown="0" dataDxfId="3">
-  <autoFilter ref="A1:C9" xr:uid="{FAEA9955-847F-4766-AEEA-E6C31E526FE4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FAEA9955-847F-4766-AEEA-E6C31E526FE4}" name="plantilla_recaudaciones" displayName="plantilla_recaudaciones" ref="A1:C10" tableType="queryTable" totalsRowShown="0" dataDxfId="3">
+  <autoFilter ref="A1:C10" xr:uid="{FAEA9955-847F-4766-AEEA-E6C31E526FE4}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{8E4094FF-6CA4-4D64-891C-B03FBD13327B}" uniqueName="1" name="cod_concepto" queryTableFieldId="1" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{8CBB881F-B6AA-4E0E-9DBD-82E91922998C}" uniqueName="2" name="concepto" queryTableFieldId="2" dataDxfId="1"/>
@@ -534,7 +537,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2FA9CFB-C370-4C4E-A53D-3878D6957A87}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -626,15 +629,24 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="E9" s="5"/>
+      <c r="C10" s="2"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="QrPcCqifQWbczzO0u36gpcjPYg5MugbieQT8po4hGRSz2UocjgB3js62CO+XmPMmhMcNvGe8aTthmwz3X9RaBg==" saltValue="FPHx2vcEJo8Ov6beY1SUTw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="nFaN8hxHg0HA+aJ+whLWIBtLFUFhiN73Rx0sn9rmp7tmi3UNdPMeo6dEfeY7PyCOm0SRemjk/kbv0785uvs3Vw==" saltValue="PpOF4y0b/GIADJ0QWVTEaw==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <dataValidations count="1">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error de carga" error="Valor inválido. Verifique que sea un número decimal, con solo dos decimales y que la fila admita carga." sqref="C2:C9" xr:uid="{79F2BA6A-0638-449B-B30D-BF30318C7A95}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error de carga" error="Valor inválido. Verifique que sea un número decimal, con solo dos decimales y que la fila admita carga." sqref="C2:C10" xr:uid="{79F2BA6A-0638-449B-B30D-BF30318C7A95}">
       <formula1>OR(   C2="",   AND(     ISNUMBER(C2),     C2&gt;=0,     ROUND(C2,2)=C2   ) )</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>